<commit_message>
small changes to formula - mainly to send to desktop
</commit_message>
<xml_diff>
--- a/data/DemographicsData.xlsx
+++ b/data/DemographicsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hendrik/git/AAU/dronesSpeed/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7598EDA6-D63E-3F4F-B2BC-AB9F29ED2596}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10B2DF0-5A68-7B4D-A9E9-275D2C458E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="640" windowWidth="25040" windowHeight="14040" xr2:uid="{7A8670BD-441F-9443-AE70-8541B73AE3D7}"/>
+    <workbookView xWindow="20" yWindow="640" windowWidth="25040" windowHeight="14040" xr2:uid="{7A8670BD-441F-9443-AE70-8541B73AE3D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>0.400000000000000</t>
   </si>
   <si>
-    <t>Precision Rate</t>
-  </si>
-  <si>
     <t>RecallRate</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>PID</t>
+  </si>
+  <si>
+    <t>PrecisionRate</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,19 +455,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>

</xml_diff>